<commit_message>
daily entry + correcting data analysis
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/Crizotinib_only/Crizonitib IC50 Assay 4 + Selumetinib Assay 1.xlsx
+++ b/Raw_SRB_data/Crizotinib_only/Crizonitib IC50 Assay 4 + Selumetinib Assay 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Priyal Dass\Documents\GitHub\PD_Lab_book\Raw_SRB_data\Crizotinib_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -378,7 +378,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H20" sqref="H20:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,15 +811,15 @@
         <v>1.0973333333333335</v>
       </c>
       <c r="C20" s="4">
-        <f>(B20/B19*C19)</f>
-        <v>97.511848341232238</v>
+        <f>(B20/1.125333*C19)</f>
+        <v>97.511877225082131</v>
       </c>
       <c r="G20">
         <v>0.98133333333333328</v>
       </c>
       <c r="H20" s="4">
-        <f>G20/G19*H19</f>
-        <v>89.728741237427613</v>
+        <f>G20/1.093667*H19</f>
+        <v>89.728713889450191</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -827,15 +827,15 @@
         <v>1.0443333333333333</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" ref="C21:C28" si="2">(B21/B20*C20)</f>
-        <v>92.802132701421797</v>
+        <f t="shared" ref="C21:C28" si="2">(B21/1.125333*C20)</f>
+        <v>90.493128506904867</v>
       </c>
       <c r="G21">
         <v>0.92733333333333334</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" ref="H21:H29" si="3">G21/G20*H20</f>
-        <v>84.79122218835721</v>
+        <f t="shared" ref="H21:H28" si="3">G21/1.093667*H20</f>
+        <v>76.082049972081833</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -844,14 +844,14 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="2"/>
-        <v>78.376777251184834</v>
+        <v>70.925618766258609</v>
       </c>
       <c r="G22">
         <v>0.71499999999999997</v>
       </c>
       <c r="H22" s="4">
         <f t="shared" si="3"/>
-        <v>65.376409631209995</v>
+        <v>49.739697485650119</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -860,14 +860,14 @@
       </c>
       <c r="C23" s="4">
         <f t="shared" si="2"/>
-        <v>60.66350710900474</v>
+        <v>43.025980527037369</v>
       </c>
       <c r="G23">
         <v>0.59633333333333338</v>
       </c>
       <c r="H23" s="4">
         <f t="shared" si="3"/>
-        <v>54.526059128314543</v>
+        <v>27.121088595165947</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -876,14 +876,14 @@
       </c>
       <c r="C24" s="4">
         <f t="shared" si="2"/>
-        <v>25.533175355450233</v>
+        <v>10.985902310488305</v>
       </c>
       <c r="G24">
         <v>0.40166666666666667</v>
       </c>
       <c r="H24" s="4">
         <f t="shared" si="3"/>
-        <v>36.72660774154221</v>
+        <v>9.9606527877239195</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -892,14 +892,14 @@
       </c>
       <c r="C25" s="4">
         <f t="shared" si="2"/>
-        <v>15.313981042654028</v>
+        <v>1.6823794955278282</v>
       </c>
       <c r="G25">
         <v>0.34966666666666663</v>
       </c>
       <c r="H25" s="4">
         <f t="shared" si="3"/>
-        <v>31.971959768363298</v>
+        <v>3.1846149313341847</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -908,14 +908,14 @@
       </c>
       <c r="C26" s="4">
         <f t="shared" si="2"/>
-        <v>12.973933649289103</v>
+        <v>0.21827086413271712</v>
       </c>
       <c r="G26">
         <v>0.26233333333333336</v>
       </c>
       <c r="H26" s="4">
         <f t="shared" si="3"/>
-        <v>23.986589454434625</v>
+        <v>0.76388027646440937</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -924,14 +924,14 @@
       </c>
       <c r="C27" s="4">
         <f t="shared" si="2"/>
-        <v>9.2120853080568743</v>
+        <v>2.0107304162493837E-2</v>
       </c>
       <c r="G27">
         <v>0.18600000000000003</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="3"/>
-        <v>17.007010057909177</v>
+        <v>0.12991315585308888</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -940,14 +940,14 @@
       </c>
       <c r="C28" s="4">
         <f t="shared" si="2"/>
-        <v>7.5533175355450259</v>
+        <v>1.5187689811033502E-3</v>
       </c>
       <c r="G28">
         <v>0.16833333333333333</v>
       </c>
       <c r="H28" s="4">
         <f t="shared" si="3"/>
-        <v>15.391648887534288</v>
+        <v>1.9995770713209137E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>